<commit_message>
feat: mejorar procesamiento de OCR y limpieza de texto en archivos PDF
</commit_message>
<xml_diff>
--- a/cargaRGM_final.xlsx
+++ b/cargaRGM_final.xlsx
@@ -493,22 +493,22 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>126-2023-MPH/A</t>
+          <t>41-2025-MPH/GM</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
+          <t>APROBAR la Liquidación Física y Financiera (con fines de verificación de cumplimiento de metas) del Proyecto: 2615348 “MEJORAMIENTO Y AMPLIACIÓN DE LOS SERVICIOS OPERATIVOS O MISIONALES INSTITUCIONALE</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
           <t>APROBAR la Liquidación Física y Financiera (con fines de verificación de cumplimiento de metas) del Proyecto: 2615348 “MEJORAMIENTO Y AMPLIACIÓN DE LOS SERVICIOS OPERATIVOS O MISIONALES INSTITUCIONALES EN LA SUBGERENCIA DE JUVENTUD, EDUCACIÓN Y DEPORTE DE LA MUNICIPALIDAD PROVINCIAL DE HUAMANGA DEL DISTRITO DE AYACUCHO DE LA PROVINCIA DE HUAMANGA DEL DEPARTAMENTO DE AYACUCHO”, ejecutado bajo la modalidad de Administración Directa, durante el ejercicio presupuestal del año 2023, de acuerdo al detalle que se consigna en la parte considerativa de la presente Resolución.</t>
         </is>
       </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>APROBAR la Liquidación Física y Financiera (con fines de verificación de cumplimiento de metas) del Proyecto: 2615348 “MEJORAMIENTO Y AMPLIACIÓN DE LOS SERVICIOS OPERATIVOS O MISIONALES INSTITUCIONALES EN LA SUBGERENCIA DE JUVENTUD, EDUCACIÓN Y DEPORTE DE LA MUNICIPALIDAD PROVINCIAL DE HUAMANGA DEL DISTRITO DE AYACUCHO DE LA PROVINCIA DE HUAMANGA DEL DEPARTAMENTO DE AYACUCHO”, ejecutado bajo la modalidad de Administración Directa, durante el ejercicio presupuestal del año 2023, de acuerdo al detalle que se consigna en la parte considerativa de la presente Resolución.</t>
-        </is>
-      </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>03/01/2025</t>
+          <t>03/09/2025</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
@@ -524,13 +524,13 @@
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>RESOLUCION 126-2023-MPH/A</t>
+          <t>RESOLUCION 41-2025-MPH/GM</t>
         </is>
       </c>
       <c r="I2" t="inlineStr"/>
       <c r="J2" t="inlineStr">
         <is>
-          <t>Archivo PDF (OCR:Sí) - 126-2023-MPH/A</t>
+          <t>Documento 41-2025-MPH/GM</t>
         </is>
       </c>
       <c r="K2" t="inlineStr">

</xml_diff>

<commit_message>
feat: Implement robust PDF processing with logging, enhanced OCR, improved resolution title extraction, and add a date formatting utility.
</commit_message>
<xml_diff>
--- a/cargaRGM_final.xlsx
+++ b/cargaRGM_final.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K2"/>
+  <dimension ref="A1:L8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -489,31 +489,36 @@
           <t>RUTA TEMP</t>
         </is>
       </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>OCR usado</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>41-2025-MPH/GM</t>
+          <t>431-2025-MPH</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>APROBAR la Liquidación Física y Financiera (con fines de verificación de cumplimiento de metas) del Proyecto: 2615348 “MEJORAMIENTO Y AMPLIACIÓN DE LOS SERVICIOS OPERATIVOS O MISIONALES INSTITUCIONALE</t>
+          <t>;</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>APROBAR la Liquidación Física y Financiera (con fines de verificación de cumplimiento de metas) del Proyecto: 2615348 “MEJORAMIENTO Y AMPLIACIÓN DE LOS SERVICIOS OPERATIVOS O MISIONALES INSTITUCIONALES EN LA SUBGERENCIA DE JUVENTUD, EDUCACIÓN Y DEPORTE DE LA MUNICIPALIDAD PROVINCIAL DE HUAMANGA DEL DISTRITO DE AYACUCHO DE LA PROVINCIA DE HUAMANGA DEL DEPARTAMENTO DE AYACUCHO”, ejecutado bajo la modalidad de Administración Directa, durante el ejercicio presupuestal del año 2023, de acuerdo al detalle que se consigna en la parte considerativa de la presente Resolución.</t>
+          <t>;</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>03/09/2025</t>
+          <t>05/09/2025</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>https://tustorage.municipalidad.gob.pe/archivos/documento_ejemplo.pdf</t>
+          <t>https://tustorage.municipalidad.gob.pe/archivos/documento_ejemplo copy 2.pdf</t>
         </is>
       </c>
       <c r="F2" t="n">
@@ -524,19 +529,334 @@
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>RESOLUCION 41-2025-MPH/GM</t>
+          <t>RESOLUCION 431-2025-MPH</t>
         </is>
       </c>
       <c r="I2" t="inlineStr"/>
       <c r="J2" t="inlineStr">
         <is>
-          <t>Documento 41-2025-MPH/GM</t>
+          <t>Documento 431-2025-MPH</t>
         </is>
       </c>
       <c r="K2" t="inlineStr">
         <is>
+          <t>documento_ejemplo copy 2.pdf</t>
+        </is>
+      </c>
+      <c r="L2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>431-2025-MPH</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>;</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>;</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>05/09/2025</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>https://tustorage.municipalidad.gob.pe/archivos/documento_ejemplo copy 3.pdf</t>
+        </is>
+      </c>
+      <c r="F3" t="n">
+        <v>159</v>
+      </c>
+      <c r="G3" t="n">
+        <v>54</v>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>RESOLUCION 431-2025-MPH</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr"/>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>Documento 431-2025-MPH</t>
+        </is>
+      </c>
+      <c r="K3" t="inlineStr">
+        <is>
+          <t>documento_ejemplo copy 3.pdf</t>
+        </is>
+      </c>
+      <c r="L3" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>431-2025-MPH</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>;</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>;</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>05/09/2025</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>https://tustorage.municipalidad.gob.pe/archivos/documento_ejemplo copy 4.pdf</t>
+        </is>
+      </c>
+      <c r="F4" t="n">
+        <v>159</v>
+      </c>
+      <c r="G4" t="n">
+        <v>54</v>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>RESOLUCION 431-2025-MPH</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr"/>
+      <c r="J4" t="inlineStr">
+        <is>
+          <t>Documento 431-2025-MPH</t>
+        </is>
+      </c>
+      <c r="K4" t="inlineStr">
+        <is>
+          <t>documento_ejemplo copy 4.pdf</t>
+        </is>
+      </c>
+      <c r="L4" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>431-2025-MPH</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>;</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>;</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>05/09/2025</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>https://tustorage.municipalidad.gob.pe/archivos/documento_ejemplo copy 5.pdf</t>
+        </is>
+      </c>
+      <c r="F5" t="n">
+        <v>159</v>
+      </c>
+      <c r="G5" t="n">
+        <v>54</v>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>RESOLUCION 431-2025-MPH</t>
+        </is>
+      </c>
+      <c r="I5" t="inlineStr"/>
+      <c r="J5" t="inlineStr">
+        <is>
+          <t>Documento 431-2025-MPH</t>
+        </is>
+      </c>
+      <c r="K5" t="inlineStr">
+        <is>
+          <t>documento_ejemplo copy 5.pdf</t>
+        </is>
+      </c>
+      <c r="L5" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>431-2025-MPH</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>;</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>;</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>05/09/2025</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>https://tustorage.municipalidad.gob.pe/archivos/documento_ejemplo copy 6.pdf</t>
+        </is>
+      </c>
+      <c r="F6" t="n">
+        <v>159</v>
+      </c>
+      <c r="G6" t="n">
+        <v>54</v>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>RESOLUCION 431-2025-MPH</t>
+        </is>
+      </c>
+      <c r="I6" t="inlineStr"/>
+      <c r="J6" t="inlineStr">
+        <is>
+          <t>Documento 431-2025-MPH</t>
+        </is>
+      </c>
+      <c r="K6" t="inlineStr">
+        <is>
+          <t>documento_ejemplo copy 6.pdf</t>
+        </is>
+      </c>
+      <c r="L6" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>431-2025-MPH</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>;</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>;</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>05/09/2025</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>https://tustorage.municipalidad.gob.pe/archivos/documento_ejemplo copy.pdf</t>
+        </is>
+      </c>
+      <c r="F7" t="n">
+        <v>159</v>
+      </c>
+      <c r="G7" t="n">
+        <v>54</v>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>RESOLUCION 431-2025-MPH</t>
+        </is>
+      </c>
+      <c r="I7" t="inlineStr"/>
+      <c r="J7" t="inlineStr">
+        <is>
+          <t>Documento 431-2025-MPH</t>
+        </is>
+      </c>
+      <c r="K7" t="inlineStr">
+        <is>
+          <t>documento_ejemplo copy.pdf</t>
+        </is>
+      </c>
+      <c r="L7" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>431-2025-MPH</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>;</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>;</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>05/09/2025</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>https://tustorage.municipalidad.gob.pe/archivos/documento_ejemplo.pdf</t>
+        </is>
+      </c>
+      <c r="F8" t="n">
+        <v>159</v>
+      </c>
+      <c r="G8" t="n">
+        <v>54</v>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>RESOLUCION 431-2025-MPH</t>
+        </is>
+      </c>
+      <c r="I8" t="inlineStr"/>
+      <c r="J8" t="inlineStr">
+        <is>
+          <t>Documento 431-2025-MPH</t>
+        </is>
+      </c>
+      <c r="K8" t="inlineStr">
+        <is>
           <t>documento_ejemplo.pdf</t>
         </is>
+      </c>
+      <c r="L8" t="b">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>